<commit_message>
feat: [cobrowse-0010] stable version 0.0.1
</commit_message>
<xml_diff>
--- a/sheetjs.xlsx
+++ b/sheetjs.xlsx
@@ -11,9 +11,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -44,9 +43,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -388,130 +386,187 @@
         <v>_id</v>
       </c>
       <c r="B1" t="str">
-        <v>leadId</v>
+        <v>internalField</v>
       </c>
       <c r="C1" t="str">
+        <v>name</v>
+      </c>
+      <c r="D1" t="str">
         <v>__v</v>
       </c>
-      <c r="D1" t="str">
-        <v>agree</v>
-      </c>
       <c r="E1" t="str">
-        <v>assignedTo</v>
+        <v>readableField</v>
       </c>
       <c r="F1" t="str">
-        <v>createdAt</v>
+        <v>type</v>
       </c>
       <c r="G1" t="str">
-        <v>email</v>
-      </c>
-      <c r="H1" t="str">
-        <v>followUp</v>
-      </c>
-      <c r="I1" t="str">
-        <v>nickname</v>
-      </c>
-      <c r="J1" t="str">
-        <v>phoneNumber</v>
-      </c>
-      <c r="K1" t="str">
-        <v>phoneNumberPrefix</v>
-      </c>
-      <c r="L1" t="str">
-        <v>review</v>
-      </c>
-      <c r="M1" t="str">
-        <v>status</v>
-      </c>
-      <c r="N1" t="str">
-        <v>updatedAt</v>
+        <v>checked</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="str">
-        <v>IND12345</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="b">
+        <v>email</v>
+      </c>
+      <c r="C2" t="str">
+        <v>core</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Email Id</v>
+      </c>
+      <c r="F2" t="str">
+        <v>string</v>
+      </c>
+      <c r="G2" t="b">
         <v>1</v>
-      </c>
-      <c r="E2" t="str">
-        <v>whatever@shanur.com</v>
-      </c>
-      <c r="F2" s="1">
-        <v>43995.955829907405</v>
-      </c>
-      <c r="G2" t="str">
-        <v>whatever@email.com</v>
-      </c>
-      <c r="H2" s="1">
-        <v>25569.167314675928</v>
-      </c>
-      <c r="I2" t="str">
-        <v>shanur</v>
-      </c>
-      <c r="J2" t="str">
-        <v>911112311</v>
-      </c>
-      <c r="K2" s="1">
-        <v>25569.166806608795</v>
-      </c>
-      <c r="L2" t="str">
-        <v>negative</v>
-      </c>
-      <c r="M2" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="N2" s="1">
-        <v>43995.975680717595</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="str">
-        <v>IND1234</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="b">
+        <v>nickname</v>
+      </c>
+      <c r="C3" t="str">
+        <v>core</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Nick Name</v>
+      </c>
+      <c r="F3" t="str">
+        <v>string</v>
+      </c>
+      <c r="G3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" t="str">
-        <v>whatever@shanur.com</v>
-      </c>
-      <c r="F3" s="1">
-        <v>43995.95508517361</v>
-      </c>
-      <c r="G3" t="str">
-        <v>whatever@email.com</v>
-      </c>
-      <c r="H3" s="1">
-        <v>25569.167314675928</v>
-      </c>
-      <c r="I3" t="str">
-        <v>shanur</v>
-      </c>
-      <c r="J3" t="str">
-        <v>911112311</v>
-      </c>
-      <c r="K3" s="1">
-        <v>25569.166806608795</v>
-      </c>
-      <c r="L3" t="str">
-        <v>negative</v>
-      </c>
-      <c r="M3" t="str">
-        <v>NEW</v>
-      </c>
-      <c r="N3" s="1">
-        <v>43995.97568083333</v>
+    </row>
+    <row r="4">
+      <c r="B4" t="str">
+        <v>phoneNumber</v>
+      </c>
+      <c r="C4" t="str">
+        <v>core</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Phone Number</v>
+      </c>
+      <c r="F4" t="str">
+        <v>string</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="str">
+        <v>phoneNumberPrefix</v>
+      </c>
+      <c r="C5" t="str">
+        <v>core</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Phone Number Prefix</v>
+      </c>
+      <c r="F5" t="str">
+        <v>string</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="str">
+        <v>amount</v>
+      </c>
+      <c r="C6" t="str">
+        <v>core</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Amount</v>
+      </c>
+      <c r="F6" t="str">
+        <v>number</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="str">
+        <v>followUp</v>
+      </c>
+      <c r="C7" t="str">
+        <v>core</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="str">
+        <v>FollowUp</v>
+      </c>
+      <c r="F7" t="str">
+        <v>date</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="str">
+        <v>agree</v>
+      </c>
+      <c r="C8" t="str">
+        <v>core</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Agree</v>
+      </c>
+      <c r="F8" t="str">
+        <v>boolean</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="str">
+        <v>status</v>
+      </c>
+      <c r="C9" t="str">
+        <v>core</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Status</v>
+      </c>
+      <c r="F9" t="str">
+        <v>string</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G9"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
error handling and added a new schema, need to remove _id from rendering in the ui next
</commit_message>
<xml_diff>
--- a/sheetjs.xlsx
+++ b/sheetjs.xlsx
@@ -376,20 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -439,7 +426,7 @@
     </row>
     <row r="3">
       <c r="B3" t="str">
-        <v>title</v>
+        <v>externalId</v>
       </c>
       <c r="C3" t="str">
         <v>core</v>
@@ -451,7 +438,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <v>Title</v>
+        <v>Lead Id</v>
       </c>
       <c r="G3" t="str">
         <v>string</v>
@@ -514,12 +501,12 @@
         <v>Source</v>
       </c>
       <c r="G6" t="str">
-        <v>number</v>
+        <v>string</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="str">
-        <v>followUp</v>
+        <v>amount</v>
       </c>
       <c r="C7" t="str">
         <v>core</v>
@@ -531,15 +518,15 @@
         <v>0</v>
       </c>
       <c r="F7" t="str">
-        <v>Follow Up</v>
+        <v>Amount</v>
       </c>
       <c r="G7" t="str">
-        <v>date</v>
+        <v>number</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="str">
-        <v>lastVisited</v>
+        <v>followUp</v>
       </c>
       <c r="C8" t="str">
         <v>core</v>
@@ -551,7 +538,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="str">
-        <v>Last Visited</v>
+        <v>Follow Up</v>
       </c>
       <c r="G8" t="str">
         <v>date</v>
@@ -559,7 +546,7 @@
     </row>
     <row r="9">
       <c r="B9" t="str">
-        <v>remarks</v>
+        <v>customerEmail</v>
       </c>
       <c r="C9" t="str">
         <v>core</v>
@@ -571,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="str">
-        <v>Remarks</v>
+        <v>Customer Email</v>
       </c>
       <c r="G9" t="str">
         <v>string</v>
@@ -579,7 +566,7 @@
     </row>
     <row r="10">
       <c r="B10" t="str">
-        <v>customerEmail</v>
+        <v>phoneNumberPrefix</v>
       </c>
       <c r="C10" t="str">
         <v>core</v>
@@ -588,10 +575,10 @@
         <v>0</v>
       </c>
       <c r="E10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="str">
-        <v>Customer Email</v>
+        <v>Country Code</v>
       </c>
       <c r="G10" t="str">
         <v>string</v>
@@ -599,7 +586,7 @@
     </row>
     <row r="11">
       <c r="B11" t="str">
-        <v>mobileNumber</v>
+        <v>phoneNumber</v>
       </c>
       <c r="C11" t="str">
         <v>core</v>
@@ -619,7 +606,7 @@
     </row>
     <row r="12">
       <c r="B12" t="str">
-        <v>address</v>
+        <v>leadStatus</v>
       </c>
       <c r="C12" t="str">
         <v>core</v>
@@ -628,10 +615,10 @@
         <v>0</v>
       </c>
       <c r="E12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="str">
-        <v>Address</v>
+        <v>Lead Status</v>
       </c>
       <c r="G12" t="str">
         <v>string</v>
@@ -639,7 +626,7 @@
     </row>
     <row r="13">
       <c r="B13" t="str">
-        <v>companyName</v>
+        <v>address</v>
       </c>
       <c r="C13" t="str">
         <v>core</v>
@@ -651,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="str">
-        <v>Company</v>
+        <v>Address</v>
       </c>
       <c r="G13" t="str">
         <v>string</v>
@@ -659,7 +646,7 @@
     </row>
     <row r="14">
       <c r="B14" t="str">
-        <v>product</v>
+        <v>companyName</v>
       </c>
       <c r="C14" t="str">
         <v>core</v>
@@ -671,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="str">
-        <v>Product</v>
+        <v>Company</v>
       </c>
       <c r="G14" t="str">
         <v>string</v>
@@ -679,7 +666,7 @@
     </row>
     <row r="15">
       <c r="B15" t="str">
-        <v>geoLocation</v>
+        <v>remarks</v>
       </c>
       <c r="C15" t="str">
         <v>core</v>
@@ -691,15 +678,15 @@
         <v>0</v>
       </c>
       <c r="F15" t="str">
-        <v>Geo Location</v>
+        <v>Remarks</v>
       </c>
       <c r="G15" t="str">
-        <v>geo</v>
+        <v>string</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="str">
-        <v>bucket</v>
+        <v>product</v>
       </c>
       <c r="C16" t="str">
         <v>core</v>
@@ -711,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="str">
-        <v>Bucket</v>
+        <v>Product</v>
       </c>
       <c r="G16" t="str">
         <v>string</v>
@@ -719,7 +706,7 @@
     </row>
     <row r="17">
       <c r="B17" t="str">
-        <v>agencyLocation</v>
+        <v>geoLocation</v>
       </c>
       <c r="C17" t="str">
         <v>core</v>
@@ -731,10 +718,10 @@
         <v>0</v>
       </c>
       <c r="F17" t="str">
-        <v>Agency Location</v>
+        <v>Geo Location</v>
       </c>
       <c r="G17" t="str">
-        <v>string</v>
+        <v>geo</v>
       </c>
     </row>
     <row r="18">
@@ -759,7 +746,7 @@
     </row>
     <row r="19">
       <c r="B19" t="str">
-        <v>circle</v>
+        <v>bucket</v>
       </c>
       <c r="C19" t="str">
         <v>core</v>
@@ -768,10 +755,10 @@
         <v>0</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="str">
-        <v>Circle</v>
+        <v>Bucket</v>
       </c>
       <c r="G19" t="str">
         <v>string</v>
@@ -779,7 +766,7 @@
     </row>
     <row r="20">
       <c r="B20" t="str">
-        <v>district</v>
+        <v>pinCode</v>
       </c>
       <c r="C20" t="str">
         <v>core</v>
@@ -788,10 +775,10 @@
         <v>0</v>
       </c>
       <c r="E20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="str">
-        <v>District</v>
+        <v>Pin Code</v>
       </c>
       <c r="G20" t="str">
         <v>string</v>
@@ -799,7 +786,7 @@
     </row>
     <row r="21">
       <c r="B21" t="str">
-        <v>pinCode</v>
+        <v>createdAt</v>
       </c>
       <c r="C21" t="str">
         <v>core</v>
@@ -811,15 +798,15 @@
         <v>0</v>
       </c>
       <c r="F21" t="str">
-        <v>Pin Code</v>
+        <v>Created At</v>
       </c>
       <c r="G21" t="str">
-        <v>string</v>
+        <v>date</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="str">
-        <v>workPhone</v>
+        <v>updatedAt</v>
       </c>
       <c r="C22" t="str">
         <v>core</v>
@@ -828,138 +815,75 @@
         <v>0</v>
       </c>
       <c r="E22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="str">
-        <v>Work Phone</v>
+        <v>Updated At</v>
       </c>
       <c r="G22" t="str">
-        <v>string</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="str">
-        <v>homePhone</v>
-      </c>
-      <c r="C23" t="str">
-        <v>core</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23" t="b">
-        <v>0</v>
-      </c>
-      <c r="F23" t="str">
-        <v>Home Phone</v>
-      </c>
-      <c r="G23" t="str">
-        <v>string</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="str">
-        <v>state</v>
-      </c>
-      <c r="C24" t="str">
-        <v>core</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" t="str">
-        <v>State</v>
-      </c>
-      <c r="G24" t="str">
-        <v>string</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" t="str">
-        <v>city</v>
-      </c>
-      <c r="C25" t="str">
-        <v>core</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" t="str">
-        <v>City</v>
-      </c>
-      <c r="G25" t="str">
-        <v>string</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" t="str">
-        <v>leadStatus</v>
-      </c>
-      <c r="C26" t="str">
-        <v>core</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" t="str">
-        <v>Lead Status</v>
-      </c>
-      <c r="G26" t="str">
-        <v>string</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" t="str">
-        <v>createdAt</v>
-      </c>
-      <c r="C27" t="str">
-        <v>core</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27" t="b">
-        <v>0</v>
-      </c>
-      <c r="F27" t="str">
-        <v>Created At</v>
-      </c>
-      <c r="G27" t="str">
-        <v>date</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" t="str">
-        <v>updatedAt</v>
-      </c>
-      <c r="C28" t="str">
-        <v>core</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28" t="b">
-        <v>0</v>
-      </c>
-      <c r="F28" t="str">
-        <v>Updated At</v>
-      </c>
-      <c r="G28" t="str">
         <v>date</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G28"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G22"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>_id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>internalField</v>
+      </c>
+      <c r="C1" t="str">
+        <v>name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>__v</v>
+      </c>
+      <c r="E1" t="str">
+        <v>checked</v>
+      </c>
+      <c r="F1" t="str">
+        <v>readableField</v>
+      </c>
+      <c r="G1" t="str">
+        <v>type</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="str">
+        <v>_id</v>
+      </c>
+      <c r="C2" t="str">
+        <v>core</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="str">
+        <v>CRM Id</v>
+      </c>
+      <c r="G2" t="str">
+        <v>string</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
small refactoring work done
</commit_message>
<xml_diff>
--- a/sheetjs.xlsx
+++ b/sheetjs.xlsx
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -406,7 +406,7 @@
     </row>
     <row r="2">
       <c r="B2" t="str">
-        <v>email</v>
+        <v>_id</v>
       </c>
       <c r="C2" t="str">
         <v>core</v>
@@ -415,10 +415,10 @@
         <v>0</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="str">
-        <v>Email Id</v>
+        <v>CRM Id</v>
       </c>
       <c r="G2" t="str">
         <v>string</v>
@@ -426,7 +426,7 @@
     </row>
     <row r="3">
       <c r="B3" t="str">
-        <v>externalId</v>
+        <v>email</v>
       </c>
       <c r="C3" t="str">
         <v>core</v>
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <v>Lead Id</v>
+        <v>Email Id</v>
       </c>
       <c r="G3" t="str">
         <v>string</v>
@@ -446,7 +446,7 @@
     </row>
     <row r="4">
       <c r="B4" t="str">
-        <v>firstName</v>
+        <v>externalId</v>
       </c>
       <c r="C4" t="str">
         <v>core</v>
@@ -458,7 +458,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="str">
-        <v>First Name</v>
+        <v>Lead Id</v>
       </c>
       <c r="G4" t="str">
         <v>string</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="5">
       <c r="B5" t="str">
-        <v>lastName</v>
+        <v>firstName</v>
       </c>
       <c r="C5" t="str">
         <v>core</v>
@@ -475,10 +475,10 @@
         <v>0</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="str">
-        <v>Last Name</v>
+        <v>First Name</v>
       </c>
       <c r="G5" t="str">
         <v>string</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="6">
       <c r="B6" t="str">
-        <v>source</v>
+        <v>lastName</v>
       </c>
       <c r="C6" t="str">
         <v>core</v>
@@ -495,10 +495,10 @@
         <v>0</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="str">
-        <v>Source</v>
+        <v>Last Name</v>
       </c>
       <c r="G6" t="str">
         <v>string</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="7">
       <c r="B7" t="str">
-        <v>amount</v>
+        <v>source</v>
       </c>
       <c r="C7" t="str">
         <v>core</v>
@@ -515,18 +515,18 @@
         <v>0</v>
       </c>
       <c r="E7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="str">
-        <v>Amount</v>
+        <v>Source</v>
       </c>
       <c r="G7" t="str">
-        <v>number</v>
+        <v>string</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="str">
-        <v>followUp</v>
+        <v>amount</v>
       </c>
       <c r="C8" t="str">
         <v>core</v>
@@ -538,15 +538,15 @@
         <v>0</v>
       </c>
       <c r="F8" t="str">
-        <v>Follow Up</v>
+        <v>Amount</v>
       </c>
       <c r="G8" t="str">
-        <v>date</v>
+        <v>number</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="str">
-        <v>customerEmail</v>
+        <v>followUp</v>
       </c>
       <c r="C9" t="str">
         <v>core</v>
@@ -558,15 +558,15 @@
         <v>0</v>
       </c>
       <c r="F9" t="str">
-        <v>Customer Email</v>
+        <v>Follow Up</v>
       </c>
       <c r="G9" t="str">
-        <v>string</v>
+        <v>date</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="str">
-        <v>phoneNumberPrefix</v>
+        <v>customerEmail</v>
       </c>
       <c r="C10" t="str">
         <v>core</v>
@@ -575,10 +575,10 @@
         <v>0</v>
       </c>
       <c r="E10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="str">
-        <v>Country Code</v>
+        <v>Customer Email</v>
       </c>
       <c r="G10" t="str">
         <v>string</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="11">
       <c r="B11" t="str">
-        <v>phoneNumber</v>
+        <v>phoneNumberPrefix</v>
       </c>
       <c r="C11" t="str">
         <v>core</v>
@@ -595,10 +595,10 @@
         <v>0</v>
       </c>
       <c r="E11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="str">
-        <v>Mobile Number</v>
+        <v>Country Code</v>
       </c>
       <c r="G11" t="str">
         <v>string</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="12">
       <c r="B12" t="str">
-        <v>leadStatus</v>
+        <v>phoneNumber</v>
       </c>
       <c r="C12" t="str">
         <v>core</v>
@@ -615,10 +615,10 @@
         <v>0</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="str">
-        <v>Lead Status</v>
+        <v>Mobile Number</v>
       </c>
       <c r="G12" t="str">
         <v>string</v>
@@ -626,7 +626,7 @@
     </row>
     <row r="13">
       <c r="B13" t="str">
-        <v>address</v>
+        <v>leadStatus</v>
       </c>
       <c r="C13" t="str">
         <v>core</v>
@@ -638,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="str">
-        <v>Address</v>
+        <v>Lead Status</v>
       </c>
       <c r="G13" t="str">
         <v>string</v>
@@ -646,7 +646,7 @@
     </row>
     <row r="14">
       <c r="B14" t="str">
-        <v>companyName</v>
+        <v>address</v>
       </c>
       <c r="C14" t="str">
         <v>core</v>
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="str">
-        <v>Company</v>
+        <v>Address</v>
       </c>
       <c r="G14" t="str">
         <v>string</v>
@@ -666,7 +666,7 @@
     </row>
     <row r="15">
       <c r="B15" t="str">
-        <v>remarks</v>
+        <v>companyName</v>
       </c>
       <c r="C15" t="str">
         <v>core</v>
@@ -675,10 +675,10 @@
         <v>0</v>
       </c>
       <c r="E15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="str">
-        <v>Remarks</v>
+        <v>Company</v>
       </c>
       <c r="G15" t="str">
         <v>string</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="16">
       <c r="B16" t="str">
-        <v>product</v>
+        <v>remarks</v>
       </c>
       <c r="C16" t="str">
         <v>core</v>
@@ -695,10 +695,10 @@
         <v>0</v>
       </c>
       <c r="E16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="str">
-        <v>Product</v>
+        <v>Remarks</v>
       </c>
       <c r="G16" t="str">
         <v>string</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="17">
       <c r="B17" t="str">
-        <v>geoLocation</v>
+        <v>product</v>
       </c>
       <c r="C17" t="str">
         <v>core</v>
@@ -715,18 +715,18 @@
         <v>0</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="str">
-        <v>Geo Location</v>
+        <v>Product</v>
       </c>
       <c r="G17" t="str">
-        <v>geo</v>
+        <v>string</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="str">
-        <v>operationalArea</v>
+        <v>geoLocation</v>
       </c>
       <c r="C18" t="str">
         <v>core</v>
@@ -735,18 +735,18 @@
         <v>0</v>
       </c>
       <c r="E18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="str">
-        <v>Operational Area</v>
+        <v>Geo Location</v>
       </c>
       <c r="G18" t="str">
-        <v>string</v>
+        <v>geo</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="str">
-        <v>bucket</v>
+        <v>operationalArea</v>
       </c>
       <c r="C19" t="str">
         <v>core</v>
@@ -758,7 +758,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="str">
-        <v>Bucket</v>
+        <v>Operational Area</v>
       </c>
       <c r="G19" t="str">
         <v>string</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="20">
       <c r="B20" t="str">
-        <v>pinCode</v>
+        <v>bucket</v>
       </c>
       <c r="C20" t="str">
         <v>core</v>
@@ -775,10 +775,10 @@
         <v>0</v>
       </c>
       <c r="E20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="str">
-        <v>Pin Code</v>
+        <v>Bucket</v>
       </c>
       <c r="G20" t="str">
         <v>string</v>
@@ -786,7 +786,7 @@
     </row>
     <row r="21">
       <c r="B21" t="str">
-        <v>createdAt</v>
+        <v>pinCode</v>
       </c>
       <c r="C21" t="str">
         <v>core</v>
@@ -798,15 +798,15 @@
         <v>0</v>
       </c>
       <c r="F21" t="str">
-        <v>Created At</v>
+        <v>Pin Code</v>
       </c>
       <c r="G21" t="str">
-        <v>date</v>
+        <v>string</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="str">
-        <v>updatedAt</v>
+        <v>createdAt</v>
       </c>
       <c r="C22" t="str">
         <v>core</v>
@@ -818,72 +818,48 @@
         <v>0</v>
       </c>
       <c r="F22" t="str">
-        <v>Updated At</v>
+        <v>Created At</v>
       </c>
       <c r="G22" t="str">
         <v>date</v>
       </c>
     </row>
+    <row r="23">
+      <c r="B23" t="str">
+        <v>updatedAt</v>
+      </c>
+      <c r="C23" t="str">
+        <v>core</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" t="str">
+        <v>Updated At</v>
+      </c>
+      <c r="G23" t="str">
+        <v>date</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G22"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G23"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>_id</v>
-      </c>
-      <c r="B1" t="str">
-        <v>internalField</v>
-      </c>
-      <c r="C1" t="str">
-        <v>name</v>
-      </c>
-      <c r="D1" t="str">
-        <v>__v</v>
-      </c>
-      <c r="E1" t="str">
-        <v>checked</v>
-      </c>
-      <c r="F1" t="str">
-        <v>readableField</v>
-      </c>
-      <c r="G1" t="str">
-        <v>type</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" t="str">
-        <v>_id</v>
-      </c>
-      <c r="C2" t="str">
-        <v>core</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="str">
-        <v>CRM Id</v>
-      </c>
-      <c r="G2" t="str">
-        <v>string</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fetch next lead fix, splitting string if options contains fields seperated by commas
</commit_message>
<xml_diff>
--- a/sheetjs.xlsx
+++ b/sheetjs.xlsx
@@ -11,9 +11,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -44,9 +43,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,120 +376,533 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="str">
+      <c r="A1" t="str">
         <v>_id</v>
       </c>
-      <c r="B1" s="1" t="str">
+      <c r="B1" t="str">
         <v>internalField</v>
       </c>
-      <c r="C1" s="1" t="str">
+      <c r="C1" t="str">
         <v>name</v>
       </c>
-      <c r="D1" s="1" t="str">
+      <c r="D1" t="str">
         <v>__v</v>
       </c>
+      <c r="E1" t="str">
+        <v>checked</v>
+      </c>
+      <c r="F1" t="str">
+        <v>readableField</v>
+      </c>
+      <c r="G1" t="str">
+        <v>type</v>
+      </c>
+      <c r="H1" t="str">
+        <v>options</v>
+      </c>
     </row>
     <row r="2">
-      <c r="C2" s="1" t="str">
-        <v>spec-v4</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
+      <c r="B2" t="str">
+        <v>_id</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="str">
+        <v>CRM Id</v>
+      </c>
+      <c r="G2" t="str">
+        <v>string</v>
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="1" t="str">
-        <v>spec-v4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
+      <c r="B3" t="str">
+        <v>email</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Email Id</v>
+      </c>
+      <c r="G3" t="str">
+        <v>string</v>
       </c>
     </row>
     <row r="4">
-      <c r="C4" s="1" t="str">
-        <v>spec-v4</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
+      <c r="B4" t="str">
+        <v>externalId</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Lead Id</v>
+      </c>
+      <c r="G4" t="str">
+        <v>string</v>
       </c>
     </row>
     <row r="5">
-      <c r="C5" s="1" t="str">
-        <v>spec-v4</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
+      <c r="B5" t="str">
+        <v>firstName</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
+        <v>First Name</v>
+      </c>
+      <c r="G5" t="str">
+        <v>string</v>
       </c>
     </row>
     <row r="6">
-      <c r="C6" s="1" t="str">
-        <v>spec-v4</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
+      <c r="B6" t="str">
+        <v>lastName</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="str">
+        <v>Last Name</v>
+      </c>
+      <c r="G6" t="str">
+        <v>string</v>
       </c>
     </row>
     <row r="7">
-      <c r="C7" s="1" t="str">
-        <v>spec-v4</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
+      <c r="B7" t="str">
+        <v>source</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Source</v>
+      </c>
+      <c r="G7" t="str">
+        <v>string</v>
       </c>
     </row>
     <row r="8">
-      <c r="C8" s="1" t="str">
-        <v>spec-v4</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
+      <c r="B8" t="str">
+        <v>amount</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Amount</v>
+      </c>
+      <c r="G8" t="str">
+        <v>number</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="str">
+        <v>followUp</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Follow Up</v>
+      </c>
+      <c r="G9" t="str">
+        <v>date</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="str">
+        <v>customerEmail</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Customer Email</v>
+      </c>
+      <c r="G10" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="str">
+        <v>phoneNumberPrefix</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Country Code</v>
+      </c>
+      <c r="G11" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="str">
+        <v>phoneNumber</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Mobile Number</v>
+      </c>
+      <c r="G12" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="str">
+        <v>leadStatus</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Lead Status</v>
+      </c>
+      <c r="G13" t="str">
+        <v>select</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="str">
+        <v>callDisposition</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Call Disposition</v>
+      </c>
+      <c r="G14" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="str">
+        <v>address</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Address</v>
+      </c>
+      <c r="G15" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="str">
+        <v>companyName</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="str">
+        <v>Company</v>
+      </c>
+      <c r="G16" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="str">
+        <v>remarks</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" t="str">
+        <v>Remarks</v>
+      </c>
+      <c r="G17" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="str">
+        <v>product</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Product</v>
+      </c>
+      <c r="G18" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="str">
+        <v>geoLocation</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" t="str">
+        <v>Geo Location</v>
+      </c>
+      <c r="G19" t="str">
+        <v>geo</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="str">
+        <v>operationalArea</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="str">
+        <v>Operational Area</v>
+      </c>
+      <c r="G20" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="str">
+        <v>bucket</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="str">
+        <v>Bucket</v>
+      </c>
+      <c r="G21" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="str">
+        <v>alternateMobile</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="str">
+        <v>Alternate Mobile</v>
+      </c>
+      <c r="G22" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="str">
+        <v>pinCode</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" t="str">
+        <v>Pin Code</v>
+      </c>
+      <c r="G23" t="str">
+        <v>string</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="str">
+        <v>createdAt</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" t="str">
+        <v>Created At</v>
+      </c>
+      <c r="G24" t="str">
+        <v>date</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="str">
+        <v>updatedAt</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Spec 4 with options select options upload</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" t="str">
+        <v>Updated At</v>
+      </c>
+      <c r="G25" t="str">
+        <v>date</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H25"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="str">
-        <v>_id</v>
-      </c>
-      <c r="B1" s="1" t="str">
-        <v>internalField</v>
-      </c>
-      <c r="C1" s="1" t="str">
-        <v>name</v>
-      </c>
-      <c r="D1" s="1" t="str">
-        <v>__v</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="C2" s="1" t="str">
-        <v>spec-v4</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>